<commit_message>
Add chart to ID excel file
</commit_message>
<xml_diff>
--- a/testes/ID/J5_Log_excel.xlsx
+++ b/testes/ID/J5_Log_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\androidconcurrency\testes\ID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40A2334-29E5-48CA-AECE-A90865113ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C09D8F5-89F4-4589-8606-831EEFC0D755}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12645" yWindow="2475" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="J5_Log_agreggated" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t>Image download</t>
   </si>
@@ -69,6 +69,27 @@
   </si>
   <si>
     <t>Median</t>
+  </si>
+  <si>
+    <t>Thread</t>
+  </si>
+  <si>
+    <t>IntentService</t>
+  </si>
+  <si>
+    <t>785 KB</t>
+  </si>
+  <si>
+    <t>542 KB</t>
+  </si>
+  <si>
+    <t>202 KB</t>
+  </si>
+  <si>
+    <t>60 KB</t>
+  </si>
+  <si>
+    <t>83 KB</t>
   </si>
 </sst>
 </file>
@@ -646,6 +667,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF93ADDD"/>
+      <color rgb="FFFF6565"/>
+      <color rgb="FFF2A16A"/>
+      <color rgb="FFBC8FDD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -655,6 +684,1852 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Download</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> de imagens</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Thread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="93ADDD"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$C$148,J5_Log_agreggated!$C$185,J5_Log_agreggated!$C$111,J5_Log_agreggated!$C$74,J5_Log_agreggated!$C$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>44.703125</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>90.03125</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>47.6484375</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>177.431640625</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>223.966796875</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$C$148,J5_Log_agreggated!$C$185,J5_Log_agreggated!$C$111,J5_Log_agreggated!$C$74,J5_Log_agreggated!$C$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>44.703125</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>90.03125</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>47.6484375</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>177.431640625</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>223.966796875</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$L$3:$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>60 KB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83 KB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>202 KB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>542 KB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>785 KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$L$4:$P$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>434.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>445.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>920.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1135</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E10-4E7B-97EA-D4B35664FE09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$K$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ThreadPool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF6565"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$D$148,J5_Log_agreggated!$D$185,J5_Log_agreggated!$D$111,J5_Log_agreggated!$D$74,J5_Log_agreggated!$D$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>66.765625</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>153.19140625</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>137.890625</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>173.828125</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>234.66015625</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$D$148,J5_Log_agreggated!$D$185,J5_Log_agreggated!$D$111,J5_Log_agreggated!$D$74,J5_Log_agreggated!$D$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>66.765625</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>153.19140625</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>137.890625</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>173.828125</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>234.66015625</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$L$3:$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>60 KB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83 KB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>202 KB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>542 KB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>785 KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$L$5:$P$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>433.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>462</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>648.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1203.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E10-4E7B-97EA-D4B35664FE09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$K$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HaMeR framework</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$E$148,J5_Log_agreggated!$E$185,J5_Log_agreggated!$E$111,J5_Log_agreggated!$E$74,J5_Log_agreggated!$E$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>80.71875</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>328.080078125</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>100.810546875</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>219.89453125</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>248.548828125</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$E$148,J5_Log_agreggated!$E$185,J5_Log_agreggated!$E$111,J5_Log_agreggated!$E$74,J5_Log_agreggated!$E$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>80.71875</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>328.080078125</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>100.810546875</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>219.89453125</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>248.548828125</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$L$3:$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>60 KB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83 KB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>202 KB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>542 KB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>785 KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$L$6:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>497</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>914.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1113</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7E10-4E7B-97EA-D4B35664FE09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$K$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kotlin coroutines</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$F$148,J5_Log_agreggated!$F$185,J5_Log_agreggated!$F$111,J5_Log_agreggated!$F$74,J5_Log_agreggated!$F$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>63.265625</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>77.794921875</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>96.22265625</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>101.6953125</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>147.35546875</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$F$148,J5_Log_agreggated!$F$185,J5_Log_agreggated!$F$111,J5_Log_agreggated!$F$74,J5_Log_agreggated!$F$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>63.265625</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>77.794921875</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>96.22265625</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>101.6953125</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>147.35546875</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$L$3:$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>60 KB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83 KB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>202 KB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>542 KB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>785 KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$L$7:$P$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>435.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>612.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>669.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7E10-4E7B-97EA-D4B35664FE09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$K$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AsyncTask</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F2A16A"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$G$148,J5_Log_agreggated!$G$185,J5_Log_agreggated!$G$111,J5_Log_agreggated!$G$74,J5_Log_agreggated!$G$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>28.169921875</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>36.5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>65.486328125</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>119.625</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>205.794921875</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$G$148,J5_Log_agreggated!$G$185,J5_Log_agreggated!$G$111,J5_Log_agreggated!$G$74,J5_Log_agreggated!$G$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>28.169921875</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>36.5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>65.486328125</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>119.625</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>205.794921875</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$L$3:$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>60 KB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83 KB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>202 KB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>542 KB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>785 KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$L$8:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>429.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>427.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>652.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-7E10-4E7B-97EA-D4B35664FE09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$K$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IntentService</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="BC8FDD"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$H$148,J5_Log_agreggated!$H$185,J5_Log_agreggated!$H$111,J5_Log_agreggated!$H$74,J5_Log_agreggated!$H$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>121.3828125</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>30.578125</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>99.111328125</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>198.4765625</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>221.609375</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(J5_Log_agreggated!$H$148,J5_Log_agreggated!$H$185,J5_Log_agreggated!$H$111,J5_Log_agreggated!$H$74,J5_Log_agreggated!$H$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>121.3828125</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>30.578125</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>99.111328125</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>198.4765625</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>221.609375</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$L$3:$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>60 KB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83 KB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>202 KB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>542 KB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>785 KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$L$9:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>419.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>426.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>783.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>866</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-7E10-4E7B-97EA-D4B35664FE09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="414017312"/>
+        <c:axId val="414012880"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="414017312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Tamanho</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> das imagens (KB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414012880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="414012880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Tempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414017312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>398318</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>117763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1021772</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>69273</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC19CCF0-C32F-4A7F-8F5E-09DB84B5E0F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -954,25 +2829,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H191"/>
+  <dimension ref="A1:P191"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B165" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -991,8 +2866,23 @@
       <c r="H3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1075</v>
       </c>
@@ -1011,8 +2901,26 @@
       <c r="H4">
         <v>666</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4">
+        <v>434.5</v>
+      </c>
+      <c r="M4">
+        <v>445.5</v>
+      </c>
+      <c r="N4">
+        <v>461</v>
+      </c>
+      <c r="O4">
+        <v>920.5</v>
+      </c>
+      <c r="P4">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1072</v>
       </c>
@@ -1031,8 +2939,26 @@
       <c r="H5">
         <v>685</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>412</v>
+      </c>
+      <c r="M5">
+        <v>433.5</v>
+      </c>
+      <c r="N5">
+        <v>462</v>
+      </c>
+      <c r="O5">
+        <v>648.5</v>
+      </c>
+      <c r="P5">
+        <v>1203.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1176</v>
       </c>
@@ -1051,8 +2977,26 @@
       <c r="H6">
         <v>642</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>419</v>
+      </c>
+      <c r="M6">
+        <v>436</v>
+      </c>
+      <c r="N6">
+        <v>497</v>
+      </c>
+      <c r="O6">
+        <v>914.5</v>
+      </c>
+      <c r="P6">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1037</v>
       </c>
@@ -1071,8 +3015,26 @@
       <c r="H7">
         <v>681</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>430</v>
+      </c>
+      <c r="M7">
+        <v>435.5</v>
+      </c>
+      <c r="N7">
+        <v>486</v>
+      </c>
+      <c r="O7">
+        <v>612.5</v>
+      </c>
+      <c r="P7">
+        <v>669.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>948</v>
       </c>
@@ -1091,8 +3053,26 @@
       <c r="H8">
         <v>908</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>429.5</v>
+      </c>
+      <c r="M8">
+        <v>427.5</v>
+      </c>
+      <c r="N8">
+        <v>444</v>
+      </c>
+      <c r="O8">
+        <v>652.5</v>
+      </c>
+      <c r="P8">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>1068</v>
       </c>
@@ -1111,8 +3091,26 @@
       <c r="H9">
         <v>791</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9">
+        <v>419.5</v>
+      </c>
+      <c r="M9">
+        <v>426.5</v>
+      </c>
+      <c r="N9">
+        <v>575</v>
+      </c>
+      <c r="O9">
+        <v>783.5</v>
+      </c>
+      <c r="P9">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>1980</v>
       </c>
@@ -1132,7 +3130,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>1153</v>
       </c>
@@ -1152,7 +3150,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>1105</v>
       </c>
@@ -1172,7 +3170,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>1461</v>
       </c>
@@ -1192,7 +3190,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>1291</v>
       </c>
@@ -1212,7 +3210,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>1595</v>
       </c>
@@ -1232,7 +3230,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>1583</v>
       </c>
@@ -4613,5 +6611,6 @@
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added charts to Producers-consumers excel file
</commit_message>
<xml_diff>
--- a/testes/ID/J5_Log_excel.xlsx
+++ b/testes/ID/J5_Log_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\androidconcurrency\testes\ID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C09D8F5-89F4-4589-8606-831EEFC0D755}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF62630F-385C-47A7-8D40-2C450A998A3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12645" yWindow="2475" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2831,8 +2831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B165" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="Y108" sqref="Y108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add nexus6 logs and excel tables
</commit_message>
<xml_diff>
--- a/testes/ID/J5_Log_excel.xlsx
+++ b/testes/ID/J5_Log_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\androidconcurrency\testes\ID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BB0DD4-7CE9-481D-AB8C-1A577393A125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975D0056-1F9A-41FA-A91E-56AB4290AF29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12645" yWindow="2790" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="J5_Log_agreggated" sheetId="1" r:id="rId1"/>
@@ -2832,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update ID to use standard error
</commit_message>
<xml_diff>
--- a/testes/ID/J5_Log_excel.xlsx
+++ b/testes/ID/J5_Log_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\androidconcurrency\testes\ID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975D0056-1F9A-41FA-A91E-56AB4290AF29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FD907B-87BC-47BE-AAC3-2E6D8CC2748A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="J5_Log_agreggated" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>Pigeon</t>
   </si>
   <si>
-    <t>Deviation</t>
-  </si>
-  <si>
     <t>Median</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>83 KB</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
   </si>
 </sst>
 </file>
@@ -803,19 +803,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>44.703125</c:v>
+                    <c:v>13.7554974347502</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>90.03125</c:v>
+                    <c:v>24.282379343313551</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>47.6484375</c:v>
+                    <c:v>13.66990970897807</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>177.431640625</c:v>
+                    <c:v>37.2316435441411</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>223.966796875</c:v>
+                    <c:v>47.482989513032535</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -827,19 +827,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>44.703125</c:v>
+                    <c:v>13.7554974347502</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>90.03125</c:v>
+                    <c:v>24.282379343313551</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>47.6484375</c:v>
+                    <c:v>13.66990970897807</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>177.431640625</c:v>
+                    <c:v>37.2316435441411</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>223.966796875</c:v>
+                    <c:v>47.482989513032535</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -946,19 +946,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>66.765625</c:v>
+                    <c:v>12.468023616565127</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>153.19140625</c:v>
+                    <c:v>54.050723591512899</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>137.890625</c:v>
+                    <c:v>40.647425572170754</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>173.828125</c:v>
+                    <c:v>40.21109714580485</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>234.66015625</c:v>
+                    <c:v>53.11883710695065</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -970,19 +970,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>66.765625</c:v>
+                    <c:v>12.468023616565127</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>153.19140625</c:v>
+                    <c:v>54.050723591512899</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>137.890625</c:v>
+                    <c:v>40.647425572170754</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>173.828125</c:v>
+                    <c:v>40.21109714580485</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>234.66015625</c:v>
+                    <c:v>53.11883710695065</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1089,19 +1089,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>80.71875</c:v>
+                    <c:v>15.109412789341272</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>328.080078125</c:v>
+                    <c:v>100.23354391296768</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>100.810546875</c:v>
+                    <c:v>22.328060981815266</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>219.89453125</c:v>
+                    <c:v>46.124763691588043</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>248.548828125</c:v>
+                    <c:v>60.450582312875412</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1113,19 +1113,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>80.71875</c:v>
+                    <c:v>15.109412789341272</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>328.080078125</c:v>
+                    <c:v>100.23354391296768</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>100.810546875</c:v>
+                    <c:v>22.328060981815266</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>219.89453125</c:v>
+                    <c:v>46.124763691588043</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>248.548828125</c:v>
+                    <c:v>60.450582312875412</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1232,19 +1232,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>63.265625</c:v>
+                    <c:v>13.950517391260833</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>77.794921875</c:v>
+                    <c:v>28.220991542808594</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>96.22265625</c:v>
+                    <c:v>25.288780079977517</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>101.6953125</c:v>
+                    <c:v>23.143306153349421</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>147.35546875</c:v>
+                    <c:v>33.304583483328294</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1256,19 +1256,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>63.265625</c:v>
+                    <c:v>13.950517391260833</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>77.794921875</c:v>
+                    <c:v>28.220991542808594</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>96.22265625</c:v>
+                    <c:v>25.288780079977517</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>101.6953125</c:v>
+                    <c:v>23.143306153349421</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>147.35546875</c:v>
+                    <c:v>33.304583483328294</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1375,19 +1375,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>28.169921875</c:v>
+                    <c:v>11.046226583036866</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>36.5</c:v>
+                    <c:v>10.245056833230796</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>65.486328125</c:v>
+                    <c:v>18.63853883190167</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>119.625</c:v>
+                    <c:v>30.112825474613238</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>205.794921875</c:v>
+                    <c:v>43.594510196863496</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1399,19 +1399,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>28.169921875</c:v>
+                    <c:v>11.046226583036866</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>36.5</c:v>
+                    <c:v>10.245056833230796</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>65.486328125</c:v>
+                    <c:v>18.63853883190167</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>119.625</c:v>
+                    <c:v>30.112825474613238</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>205.794921875</c:v>
+                    <c:v>43.594510196863496</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1518,19 +1518,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>121.3828125</c:v>
+                    <c:v>56.095602393261657</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>30.578125</c:v>
+                    <c:v>10.007954245772902</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>99.111328125</c:v>
+                    <c:v>19.885723642560922</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>198.4765625</c:v>
+                    <c:v>50.011505732632777</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>221.609375</c:v>
+                    <c:v>44.971506155869619</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1542,19 +1542,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>121.3828125</c:v>
+                    <c:v>56.095602393261657</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>30.578125</c:v>
+                    <c:v>10.007954245772902</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>99.111328125</c:v>
+                    <c:v>19.885723642560922</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>198.4765625</c:v>
+                    <c:v>50.011505732632777</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>221.609375</c:v>
+                    <c:v>44.971506155869619</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2832,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="F15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,19 +2868,19 @@
         <v>7</v>
       </c>
       <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
         <v>19</v>
       </c>
-      <c r="M3" t="s">
-        <v>20</v>
-      </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -2903,7 +2903,7 @@
         <v>666</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L4">
         <v>434.5</v>
@@ -3093,7 +3093,7 @@
         <v>791</v>
       </c>
       <c r="K9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L9">
         <v>419.5</v>
@@ -3637,7 +3637,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C36">
         <f>MEDIAN(C4:C35)</f>
@@ -3666,31 +3666,31 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C37">
-        <f>AVEDEV(C4:C35)</f>
-        <v>223.966796875</v>
+        <f>STDEV(C4:C35)/SQRT(COUNT(C4:C35))</f>
+        <v>47.482989513032535</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:H37" si="1">AVEDEV(D4:D35)</f>
-        <v>234.66015625</v>
+        <f t="shared" ref="D37:H37" si="1">STDEV(D4:D35)/SQRT(COUNT(D4:D35))</f>
+        <v>53.11883710695065</v>
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
-        <v>248.548828125</v>
+        <v>60.450582312875412</v>
       </c>
       <c r="F37">
         <f t="shared" si="1"/>
-        <v>147.35546875</v>
+        <v>33.304583483328294</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
-        <v>205.794921875</v>
+        <v>43.594510196863496</v>
       </c>
       <c r="H37">
         <f t="shared" si="1"/>
-        <v>221.609375</v>
+        <v>44.971506155869619</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -4372,7 +4372,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C73">
         <f>MEDIAN(C41:C72)</f>
@@ -4401,31 +4401,31 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C74">
-        <f>AVEDEV(C41:C72)</f>
-        <v>177.431640625</v>
+        <f>STDEV(C41:C72)/SQRT(COUNT(C41:C72))</f>
+        <v>37.2316435441411</v>
       </c>
       <c r="D74">
-        <f t="shared" ref="D74:H74" si="3">AVEDEV(D41:D72)</f>
-        <v>173.828125</v>
+        <f t="shared" ref="D74:H74" si="3">STDEV(D41:D72)/SQRT(COUNT(D41:D72))</f>
+        <v>40.21109714580485</v>
       </c>
       <c r="E74">
         <f t="shared" si="3"/>
-        <v>219.89453125</v>
+        <v>46.124763691588043</v>
       </c>
       <c r="F74">
         <f t="shared" si="3"/>
-        <v>101.6953125</v>
+        <v>23.143306153349421</v>
       </c>
       <c r="G74">
         <f t="shared" si="3"/>
-        <v>119.625</v>
+        <v>30.112825474613238</v>
       </c>
       <c r="H74">
         <f t="shared" si="3"/>
-        <v>198.4765625</v>
+        <v>50.011505732632777</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -5095,7 +5095,7 @@
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C110">
         <f>MEDIAN(C78:C109)</f>
@@ -5124,31 +5124,31 @@
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C111">
-        <f>AVEDEV(C78:C109)</f>
-        <v>47.6484375</v>
+        <f>STDEV(C78:C109)/SQRT(COUNT(C78:C109))</f>
+        <v>13.66990970897807</v>
       </c>
       <c r="D111">
-        <f t="shared" ref="D111:H111" si="5">AVEDEV(D78:D109)</f>
-        <v>137.890625</v>
+        <f t="shared" ref="D111:H111" si="5">STDEV(D78:D109)/SQRT(COUNT(D78:D109))</f>
+        <v>40.647425572170754</v>
       </c>
       <c r="E111">
         <f t="shared" si="5"/>
-        <v>100.810546875</v>
+        <v>22.328060981815266</v>
       </c>
       <c r="F111">
         <f t="shared" si="5"/>
-        <v>96.22265625</v>
+        <v>25.288780079977517</v>
       </c>
       <c r="G111">
         <f t="shared" si="5"/>
-        <v>65.486328125</v>
+        <v>18.63853883190167</v>
       </c>
       <c r="H111">
         <f t="shared" si="5"/>
-        <v>99.111328125</v>
+        <v>19.885723642560922</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5818,7 +5818,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C147">
         <f>MEDIAN(C115:C146)</f>
@@ -5847,31 +5847,31 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C148">
-        <f>AVEDEV(C115:C146)</f>
-        <v>44.703125</v>
+        <f>STDEV(C115:C146)/SQRT(COUNT(C115:C146))</f>
+        <v>13.7554974347502</v>
       </c>
       <c r="D148">
-        <f t="shared" ref="D148:H148" si="7">AVEDEV(D115:D146)</f>
-        <v>66.765625</v>
+        <f t="shared" ref="D148:H148" si="7">STDEV(D115:D146)/SQRT(COUNT(D115:D146))</f>
+        <v>12.468023616565127</v>
       </c>
       <c r="E148">
         <f t="shared" si="7"/>
-        <v>80.71875</v>
+        <v>15.109412789341272</v>
       </c>
       <c r="F148">
         <f t="shared" si="7"/>
-        <v>63.265625</v>
+        <v>13.950517391260833</v>
       </c>
       <c r="G148">
         <f t="shared" si="7"/>
-        <v>28.169921875</v>
+        <v>11.046226583036866</v>
       </c>
       <c r="H148">
         <f t="shared" si="7"/>
-        <v>121.3828125</v>
+        <v>56.095602393261657</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -6541,7 +6541,7 @@
     </row>
     <row r="184" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C184">
         <f>MEDIAN(C152:C183)</f>
@@ -6570,31 +6570,31 @@
     </row>
     <row r="185" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C185">
-        <f>AVEDEV(C152:C183)</f>
-        <v>90.03125</v>
+        <f>STDEV(C152:C183)/SQRT(COUNT(C152:C183))</f>
+        <v>24.282379343313551</v>
       </c>
       <c r="D185">
-        <f t="shared" ref="D185:H185" si="9">AVEDEV(D152:D183)</f>
-        <v>153.19140625</v>
+        <f t="shared" ref="D185:H185" si="9">STDEV(D152:D183)/SQRT(COUNT(D152:D183))</f>
+        <v>54.050723591512899</v>
       </c>
       <c r="E185">
         <f t="shared" si="9"/>
-        <v>328.080078125</v>
+        <v>100.23354391296768</v>
       </c>
       <c r="F185">
         <f t="shared" si="9"/>
-        <v>77.794921875</v>
+        <v>28.220991542808594</v>
       </c>
       <c r="G185">
         <f t="shared" si="9"/>
-        <v>36.5</v>
+        <v>10.245056833230796</v>
       </c>
       <c r="H185">
         <f t="shared" si="9"/>
-        <v>30.578125</v>
+        <v>10.007954245772902</v>
       </c>
     </row>
     <row r="191" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>